<commit_message>
analysis rerun on updated data
</commit_message>
<xml_diff>
--- a/data/cc_country_names_toCheck.xlsx
+++ b/data/cc_country_names_toCheck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schroeder\OneDrive - Hertie School\WZB\TRIAS-GP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D108D37-E2D8-49CC-BDA0-A76356D3EF37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870CA4B5-019A-4C74-95F6-AD24CC918E53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15720" windowHeight="7890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="177">
   <si>
     <t>regex</t>
   </si>
@@ -494,13 +494,64 @@
     <t>cocos island|keeling</t>
   </si>
   <si>
-    <t>german.?democratic.?rep|democratic.?rep.*germany|east.germany|germany.*east|\\bgdr\\b</t>
-  </si>
-  <si>
     <t>^(?=.*peo).*yemen|^(?!.*rep)(?=.*dem).*yemen|^(?=.*south).*yemen|^(?=.*aden).*yemen|^(?=.*\\bp\.?d\.?r).*yemen</t>
   </si>
   <si>
     <t>CSK</t>
+  </si>
+  <si>
+    <t>christmas island\\w*</t>
+  </si>
+  <si>
+    <t>cocos island\\w*|keeling</t>
+  </si>
+  <si>
+    <t>heard (island)?( and |[ &amp;\\/)]*)mcdonald</t>
+  </si>
+  <si>
+    <t>heard (island)?( and |[ &amp;\\/)]*)mcdonald( island\\w*)</t>
+  </si>
+  <si>
+    <t>german.?democratic.?rep|democratic.?rep.*germany|east.germany|germany[-\\ (]east|\\bgdr\\b</t>
+  </si>
+  <si>
+    <t>french.?southern( and |[ &amp;\\/)]*)antarct\\w*(lands)?</t>
+  </si>
+  <si>
+    <t>czechoslovak\\w*</t>
+  </si>
+  <si>
+    <t>british.?indian.?ocean( territor\\w*)?</t>
+  </si>
+  <si>
+    <t>netherlands.antil\\w*|dutch.antil\\w*</t>
+  </si>
+  <si>
+    <t>serbia( and |[ &amp;\\/)]*)montenegro</t>
+  </si>
+  <si>
+    <t>somaliland\\w*</t>
+  </si>
+  <si>
+    <t>south.?georgia|sandwich island\\w*|south.?georgia( and |[ &amp;\\/)]*)(the )?sandwich( island\\w*)?</t>
+  </si>
+  <si>
+    <t>tibet\\w*</t>
+  </si>
+  <si>
+    <t>(united states |u\\.?s\\.? )?minor.?outlying.?is\\w*</t>
+  </si>
+  <si>
+    <t>(?&lt;!former )yugoslav</t>
+  </si>
+  <si>
+    <t>(?&lt;!former )yugoslav\\w*</t>
+  </si>
+  <si>
+    <t>regex_capture_full</t>
+  </si>
+  <si>
+    <t>bouvet\\w*( island\\w*)?</t>
   </si>
 </sst>
 </file>
@@ -854,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:C49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1406,26 +1457,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{837F3409-DD4B-4BF3-8465-94498362408F}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="4" max="4" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1435,8 +1490,11 @@
       <c r="C2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1446,8 +1504,11 @@
       <c r="C6" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1457,8 +1518,11 @@
       <c r="C7" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1468,8 +1532,11 @@
       <c r="C9" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1479,8 +1546,11 @@
       <c r="C10" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1488,10 +1558,13 @@
         <v>155</v>
       </c>
       <c r="C11" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+      <c r="D11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1501,30 +1574,39 @@
       <c r="C12" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="C13" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>161</v>
       </c>
       <c r="C16" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1534,8 +1616,11 @@
       <c r="C23" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1545,8 +1630,11 @@
       <c r="C33" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1556,8 +1644,11 @@
       <c r="C34" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1567,8 +1658,11 @@
       <c r="C35" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1578,8 +1672,11 @@
       <c r="C37" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1589,27 +1686,36 @@
       <c r="C42" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C47" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>173</v>
       </c>
       <c r="C48" t="s">
         <v>151</v>
+      </c>
+      <c r="D48" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>